<commit_message>
read and prompt for 1 excel
</commit_message>
<xml_diff>
--- a/build/resources/main/compare1.xlsx
+++ b/build/resources/main/compare1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glebshvydkov/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/glebshvydkov/projects/personal/ai-excel-comp/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5A98A4-AD75-8446-8689-9B6A49FBFCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFB8D0A-CAF4-1644-8BCF-53ED3B6FEEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{DE354F3C-BA19-9243-93D3-E6F6FB93C293}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>d</t>
   </si>
   <si>
-    <t>cadabra</t>
-  </si>
-  <si>
     <t>June</t>
   </si>
   <si>
@@ -102,7 +99,10 @@
     <t>easdasd</t>
   </si>
   <si>
-    <t>asdasd</t>
+    <t>column_1</t>
+  </si>
+  <si>
+    <t>column_2</t>
   </si>
 </sst>
 </file>
@@ -642,89 +642,89 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>